<commit_message>
change rule and user-story
</commit_message>
<xml_diff>
--- a/Product Backlog and Burndown Chart.xlsx
+++ b/Product Backlog and Burndown Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="17300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="17295"/>
   </bookViews>
   <sheets>
     <sheet name="Base User Story List" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="BDC4" sheetId="6" r:id="rId4"/>
     <sheet name="Velocity" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="253">
   <si>
     <t>User Story</t>
     <phoneticPr fontId="1"/>
@@ -2193,6 +2193,13 @@
       <t>ヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4-3</t>
   </si>
 </sst>
 </file>
@@ -2338,7 +2345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2366,6 +2373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2471,7 +2484,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2697,6 +2710,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -2830,7 +2861,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2871,13 +2901,13 @@
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2916,7 +2946,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2957,13 +2986,13 @@
                   <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2979,11 +3008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076766584"/>
-        <c:axId val="2076772072"/>
+        <c:axId val="267811496"/>
+        <c:axId val="267810712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076766584"/>
+        <c:axId val="267811496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3011,12 +3040,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076772072"/>
+        <c:crossAx val="267810712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076772072"/>
+        <c:axId val="267810712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3050,7 +3079,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076766584"/>
+        <c:crossAx val="267811496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3141,7 +3170,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3179,22 +3207,22 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3233,7 +3261,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3271,22 +3298,22 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3302,11 +3329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076822120"/>
-        <c:axId val="2076827608"/>
+        <c:axId val="267813456"/>
+        <c:axId val="267810320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076822120"/>
+        <c:axId val="267813456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3334,12 +3361,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076827608"/>
+        <c:crossAx val="267810320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076827608"/>
+        <c:axId val="267810320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3373,7 +3400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076822120"/>
+        <c:crossAx val="267813456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3464,7 +3491,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3538,7 +3564,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3589,11 +3614,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076887976"/>
-        <c:axId val="2076893464"/>
+        <c:axId val="269932944"/>
+        <c:axId val="269934120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076887976"/>
+        <c:axId val="269932944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3621,12 +3646,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076893464"/>
+        <c:crossAx val="269934120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076893464"/>
+        <c:axId val="269934120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3660,7 +3685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076887976"/>
+        <c:crossAx val="269932944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3796,16 +3821,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.232558139534884</c:v>
+                  <c:v>0.23255813953488372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.152777777777778</c:v>
+                  <c:v>0.15277777777777776</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0972222222222222</c:v>
+                  <c:v>9.722222222222221E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.1</c:v>
@@ -3825,11 +3850,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2076945848"/>
-        <c:axId val="2076951496"/>
+        <c:axId val="269937648"/>
+        <c:axId val="269938432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2076945848"/>
+        <c:axId val="269937648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3872,7 +3897,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076951496"/>
+        <c:crossAx val="269938432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3880,7 +3905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076951496"/>
+        <c:axId val="269938432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3931,7 +3956,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076945848"/>
+        <c:crossAx val="269937648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5089,32 +5114,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="6.1640625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="6.125" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="44.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" style="7"/>
-    <col min="10" max="10" width="58.83203125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="6.1640625" style="3"/>
+    <col min="2" max="2" width="13.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="35.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="44.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.125" style="7"/>
+    <col min="10" max="10" width="58.875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="6.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" customHeight="1">
+    <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" s="30" customFormat="1" ht="26.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:10" s="30" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>157</v>
       </c>
@@ -5146,7 +5171,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" thickTop="1">
+    <row r="3" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -5174,7 +5199,7 @@
       <c r="I3" s="26"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="4" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>2.1</v>
       </c>
@@ -5202,7 +5227,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="5" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>2.2000000000000002</v>
       </c>
@@ -5230,7 +5255,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="6" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>2.31</v>
       </c>
@@ -5258,7 +5283,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="7" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>2.3199999999999998</v>
       </c>
@@ -5286,7 +5311,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="8" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>2.33</v>
       </c>
@@ -5314,7 +5339,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1">
+    <row r="9" spans="1:10" s="39" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>2.4</v>
       </c>
@@ -5342,7 +5367,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="10" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -5370,7 +5395,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" s="39" customFormat="1" ht="34.5" customHeight="1">
+    <row r="11" spans="1:10" s="39" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -5400,7 +5425,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="12" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>5</v>
       </c>
@@ -5430,7 +5455,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="13" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>6</v>
       </c>
@@ -5460,7 +5485,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="14" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>7</v>
       </c>
@@ -5490,7 +5515,7 @@
       </c>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="15" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>8</v>
       </c>
@@ -5520,7 +5545,7 @@
       </c>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="16" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>9</v>
       </c>
@@ -5550,7 +5575,7 @@
       </c>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="17" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>11</v>
       </c>
@@ -5580,7 +5605,7 @@
       </c>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="18" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>12</v>
       </c>
@@ -5610,7 +5635,7 @@
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="19" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>13</v>
       </c>
@@ -5640,7 +5665,7 @@
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="20" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>14</v>
       </c>
@@ -5670,7 +5695,7 @@
       </c>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="21" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>15</v>
       </c>
@@ -5700,7 +5725,7 @@
       </c>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" s="39" customFormat="1" ht="73.5" customHeight="1">
+    <row r="22" spans="1:10" s="39" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="10">
         <v>0</v>
@@ -5730,7 +5755,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="23" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>17</v>
       </c>
@@ -5762,7 +5787,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="24" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>16</v>
       </c>
@@ -5794,7 +5819,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="38" customFormat="1" ht="26.25" customHeight="1">
+    <row r="25" spans="1:10" s="38" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>10</v>
       </c>
@@ -5826,7 +5851,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="26" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>20</v>
       </c>
@@ -5858,7 +5883,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="38" customFormat="1" ht="26.25" customHeight="1">
+    <row r="27" spans="1:10" s="38" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>10</v>
       </c>
@@ -5890,7 +5915,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="28" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
         <v>20</v>
       </c>
@@ -5922,7 +5947,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="29" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="10">
         <v>8</v>
@@ -5950,7 +5975,7 @@
       </c>
       <c r="J29" s="63"/>
     </row>
-    <row r="30" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="30" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="10">
         <v>2</v>
@@ -5980,7 +6005,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="31" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="10">
         <v>3</v>
@@ -6010,7 +6035,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="32" spans="1:10" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="10">
         <v>3</v>
@@ -6040,7 +6065,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="33" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10">
         <v>30</v>
       </c>
@@ -6072,7 +6097,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="34" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10">
         <v>18</v>
       </c>
@@ -6104,7 +6129,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="35" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
         <v>19</v>
       </c>
@@ -6134,7 +6159,7 @@
       </c>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1">
+    <row r="36" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10"/>
       <c r="B36" s="10">
         <v>3</v>
@@ -6164,7 +6189,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="37" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="50">
         <v>21</v>
       </c>
@@ -6172,7 +6197,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="D37" s="50">
         <v>4</v>
@@ -6194,37 +6219,37 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A38" s="50">
+    <row r="38" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="84" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="79">
         <v>33</v>
       </c>
-      <c r="B38" s="50">
+      <c r="B38" s="79">
         <v>3</v>
       </c>
-      <c r="C38" s="51" t="s">
+      <c r="C38" s="80" t="s">
         <v>239</v>
       </c>
-      <c r="D38" s="50">
+      <c r="D38" s="79">
         <v>4</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="53" t="s">
+      <c r="F38" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="82" t="s">
         <v>245</v>
       </c>
-      <c r="H38" s="52" t="s">
+      <c r="H38" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="54"/>
-      <c r="J38" s="50" t="s">
+      <c r="I38" s="83"/>
+      <c r="J38" s="79" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="39" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="50">
         <v>29</v>
       </c>
@@ -6254,14 +6279,16 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="40" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="50">
         <v>25</v>
       </c>
       <c r="B40" s="50">
         <v>5</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="51" t="s">
+        <v>252</v>
+      </c>
       <c r="D40" s="50">
         <v>4</v>
       </c>
@@ -6282,7 +6309,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="41" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="41" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="50">
         <v>29</v>
       </c>
@@ -6310,7 +6337,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="42" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="50">
         <v>29</v>
       </c>
@@ -6338,7 +6365,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="43" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="50">
         <v>34</v>
       </c>
@@ -6366,7 +6393,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1">
+    <row r="44" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="55" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="50"/>
       <c r="B44" s="50">
         <v>2</v>
@@ -6388,7 +6415,7 @@
       <c r="I44" s="54"/>
       <c r="J44" s="53"/>
     </row>
-    <row r="45" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="77" customFormat="1" ht="26.25" customHeight="1">
+    <row r="45" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="77" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="72"/>
       <c r="B45" s="72"/>
       <c r="C45" s="73"/>
@@ -6404,7 +6431,7 @@
       <c r="I45" s="76"/>
       <c r="J45" s="75"/>
     </row>
-    <row r="46" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1">
+    <row r="46" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="15">
         <v>22</v>
       </c>
@@ -6428,7 +6455,7 @@
       <c r="I46" s="19"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1">
+    <row r="47" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="15">
         <v>39</v>
       </c>
@@ -6450,7 +6477,7 @@
       <c r="I47" s="19"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1">
+    <row r="48" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="15">
         <v>36</v>
       </c>
@@ -14662,7 +14689,7 @@
       <c r="XEZ48" s="2"/>
       <c r="XFB48" s="5"/>
     </row>
-    <row r="49" spans="1:10" ht="26.25" customHeight="1">
+    <row r="49" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15">
         <v>37</v>
       </c>
@@ -14686,7 +14713,7 @@
       <c r="I49" s="19"/>
       <c r="J49" s="18"/>
     </row>
-    <row r="50" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="50" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="44"/>
       <c r="B50" s="44">
         <v>5</v>
@@ -14710,7 +14737,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="51" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="44"/>
       <c r="B51" s="44"/>
       <c r="C51" s="45"/>
@@ -14732,7 +14759,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="52" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="44">
         <v>23</v>
       </c>
@@ -14758,7 +14785,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="53" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="44">
         <v>38</v>
       </c>
@@ -14780,7 +14807,7 @@
       <c r="I53" s="48"/>
       <c r="J53" s="47"/>
     </row>
-    <row r="54" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="54" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="44">
         <v>26</v>
       </c>
@@ -14804,7 +14831,7 @@
       <c r="I54" s="48"/>
       <c r="J54" s="47"/>
     </row>
-    <row r="55" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="55" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="44">
         <v>27</v>
       </c>
@@ -14828,7 +14855,7 @@
       <c r="I55" s="48"/>
       <c r="J55" s="47"/>
     </row>
-    <row r="56" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="56" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="44">
         <v>31</v>
       </c>
@@ -14852,7 +14879,7 @@
       <c r="I56" s="48"/>
       <c r="J56" s="47"/>
     </row>
-    <row r="57" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="57" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="44">
         <v>32</v>
       </c>
@@ -14876,7 +14903,7 @@
       <c r="I57" s="48"/>
       <c r="J57" s="47"/>
     </row>
-    <row r="58" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1">
+    <row r="58" spans="1:10" s="49" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="44">
         <v>35</v>
       </c>
@@ -14900,7 +14927,7 @@
       <c r="I58" s="48"/>
       <c r="J58" s="47"/>
     </row>
-    <row r="59" spans="1:10" s="71" customFormat="1" ht="26.25" customHeight="1">
+    <row r="59" spans="1:10" s="71" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="65">
         <v>24</v>
       </c>
@@ -14926,7 +14953,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="61" customFormat="1" ht="26.25" customHeight="1">
+    <row r="60" spans="1:10" s="61" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="56">
         <v>28</v>
       </c>
@@ -14973,12 +15000,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="3" width="8.83203125" style="9"/>
+    <col min="2" max="3" width="8.875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6"/>
       <c r="B1" s="8" t="s">
         <v>101</v>
@@ -14987,7 +15014,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>103</v>
       </c>
@@ -15000,7 +15027,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -15013,7 +15040,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>105</v>
       </c>
@@ -15026,7 +15053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>106</v>
       </c>
@@ -15039,7 +15066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
         <v>147</v>
       </c>
@@ -15051,7 +15078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="9" t="s">
         <v>107</v>
       </c>
@@ -15077,12 +15104,12 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="3" width="8.83203125" style="42"/>
+    <col min="2" max="3" width="8.875" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6"/>
       <c r="B1" s="40" t="s">
         <v>101</v>
@@ -15091,7 +15118,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>103</v>
       </c>
@@ -15104,7 +15131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -15117,7 +15144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>105</v>
       </c>
@@ -15130,7 +15157,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>106</v>
       </c>
@@ -15143,7 +15170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
         <v>147</v>
       </c>
@@ -15156,7 +15183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
         <v>215</v>
       </c>
@@ -15169,7 +15196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="42" t="s">
         <v>107</v>
       </c>
@@ -15195,12 +15222,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="3" width="8.83203125" style="42"/>
+    <col min="2" max="3" width="8.875" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6"/>
       <c r="B1" s="40" t="s">
         <v>101</v>
@@ -15209,49 +15236,49 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
         <v>147</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="21" t="s">
         <v>215</v>
       </c>
       <c r="B7" s="41"/>
       <c r="C7" s="40"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="42" t="s">
         <v>107</v>
       </c>
@@ -15277,19 +15304,19 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="5" width="12.875" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="23.875" customWidth="1"/>
+    <col min="9" max="9" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>138</v>
       </c>
@@ -15318,7 +15345,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="G2">
         <v>4.3</v>
       </c>
@@ -15327,7 +15354,7 @@
         <v>0.23255813953488372</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
         <v>149</v>
       </c>
@@ -15353,7 +15380,7 @@
         <v>0.15277777777777776</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
         <v>150</v>
       </c>
@@ -15379,7 +15406,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="20" t="s">
         <v>139</v>
       </c>
@@ -15408,7 +15435,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29">
+    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>162</v>
       </c>
@@ -15439,7 +15466,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>177</v>
       </c>
@@ -15457,22 +15484,22 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
         <v>214</v>
       </c>
@@ -15489,9 +15516,9 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>